<commit_message>
Add enhanced parsing and vocabulary engines
Introduces new hybrid vocabulary and enhanced parsing engines for improved large-scale and unknown word handling. Adds scalability test scripts, API integration examples, and updates perfect tense pattern detection in Rephrase_Parsing_Engine.py to better separate objects and time modifiers. Includes documentation for production deployment and updates binary data files.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元.xlsx
+++ b/training/data/例文入力元.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\例文セットDB作成システム\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A50ACA-91A0-4C90-B4A7-AE9E00964397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F325D64B-B662-4A25-A5C9-B1ACA0835D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="3930" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,19 +230,10 @@
     <t>ex022</t>
   </si>
   <si>
-    <t>Would I hold the call, please?</t>
-  </si>
-  <si>
     <t>ex023</t>
   </si>
   <si>
-    <t>Would she hold the phone, please?</t>
-  </si>
-  <si>
     <t>ex024</t>
-  </si>
-  <si>
-    <t>Would they hold the connection, please?</t>
   </si>
   <si>
     <t>ex025</t>
@@ -689,6 +680,18 @@
   </si>
   <si>
     <t>discuss</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Would you hold the call, please?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Would you hold the phone, please?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Would you hold the connection, please?</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1097,7 +1100,7 @@
   <dimension ref="A1:V245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1289,7 +1292,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1303,7 +1306,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -1317,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1331,7 +1334,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -1345,7 +1348,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1359,7 +1362,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -1373,7 +1376,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -1387,7 +1390,7 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -1401,7 +1404,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1415,7 +1418,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1429,7 +1432,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1443,7 +1446,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1457,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -1471,7 +1474,7 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
@@ -1485,7 +1488,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
         <v>55</v>
@@ -1499,7 +1502,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -1513,7 +1516,7 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1527,7 +1530,7 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -1541,7 +1544,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -1555,7 +1558,7 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
@@ -1569,7 +1572,7 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
@@ -1583,10 +1586,10 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -1594,13 +1597,13 @@
         <v>5004</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>214</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="4"/>
@@ -1610,13 +1613,13 @@
         <v>5004</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1624,13 +1627,13 @@
         <v>5004</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -1638,13 +1641,13 @@
         <v>5004</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -1652,13 +1655,13 @@
         <v>5004</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -1666,13 +1669,13 @@
         <v>5004</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -1680,13 +1683,13 @@
         <v>5004</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -1694,13 +1697,13 @@
         <v>5004</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -1708,13 +1711,13 @@
         <v>5004</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V37" s="4"/>
     </row>
@@ -1723,13 +1726,13 @@
         <v>5004</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -1737,13 +1740,13 @@
         <v>5004</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -1751,13 +1754,13 @@
         <v>5004</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -1765,13 +1768,13 @@
         <v>5004</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -1779,13 +1782,13 @@
         <v>5004</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
@@ -1793,13 +1796,13 @@
         <v>5004</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -1807,13 +1810,13 @@
         <v>5004</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -1821,13 +1824,13 @@
         <v>5004</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -1835,13 +1838,13 @@
         <v>5004</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -1849,13 +1852,13 @@
         <v>5004</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -1863,13 +1866,13 @@
         <v>5004</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -1877,13 +1880,13 @@
         <v>5004</v>
       </c>
       <c r="B49" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -1891,13 +1894,13 @@
         <v>5004</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
@@ -1905,13 +1908,13 @@
         <v>5004</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D51" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -1919,13 +1922,13 @@
         <v>5004</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -1933,13 +1936,13 @@
         <v>5004</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -1947,13 +1950,13 @@
         <v>5004</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D54" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
@@ -1961,13 +1964,13 @@
         <v>5004</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D55" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
@@ -1975,13 +1978,13 @@
         <v>5004</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="V56" s="4"/>
     </row>
@@ -1990,13 +1993,13 @@
         <v>5004</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D57" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -2004,13 +2007,13 @@
         <v>5004</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D58" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -2018,13 +2021,13 @@
         <v>5004</v>
       </c>
       <c r="B59" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
@@ -2032,13 +2035,13 @@
         <v>5004</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C60" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D60" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
@@ -2046,13 +2049,13 @@
         <v>5004</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D61" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -2060,13 +2063,13 @@
         <v>5004</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C62" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D62" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -2074,13 +2077,13 @@
         <v>5004</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C63" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D63" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -2088,13 +2091,13 @@
         <v>5004</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2102,13 +2105,13 @@
         <v>5004</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2116,13 +2119,13 @@
         <v>5004</v>
       </c>
       <c r="B66" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C66" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2130,13 +2133,13 @@
         <v>5004</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2144,13 +2147,13 @@
         <v>5004</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2158,13 +2161,13 @@
         <v>5004</v>
       </c>
       <c r="B69" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D69" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2172,13 +2175,13 @@
         <v>5004</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D70" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2186,13 +2189,13 @@
         <v>5004</v>
       </c>
       <c r="B71" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2200,13 +2203,13 @@
         <v>5004</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C72" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D72" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2214,13 +2217,13 @@
         <v>5004</v>
       </c>
       <c r="B73" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D73" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2228,13 +2231,13 @@
         <v>5004</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D74" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2242,13 +2245,13 @@
         <v>5004</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D75" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2256,13 +2259,13 @@
         <v>5004</v>
       </c>
       <c r="B76" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C76" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D76" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2270,13 +2273,13 @@
         <v>5004</v>
       </c>
       <c r="B77" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D77" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2284,13 +2287,13 @@
         <v>5004</v>
       </c>
       <c r="B78" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D78" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2298,13 +2301,13 @@
         <v>5004</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D79" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2312,13 +2315,13 @@
         <v>5004</v>
       </c>
       <c r="B80" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.2">
@@ -2326,13 +2329,13 @@
         <v>5004</v>
       </c>
       <c r="B81" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C81" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.2">
@@ -2340,13 +2343,13 @@
         <v>5004</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C82" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D82" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.2">
@@ -2354,13 +2357,13 @@
         <v>5004</v>
       </c>
       <c r="B83" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C83" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D83" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
@@ -2368,13 +2371,13 @@
         <v>5004</v>
       </c>
       <c r="B84" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C84" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D84" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.2">
@@ -2382,13 +2385,13 @@
         <v>5004</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C85" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D85" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
@@ -2396,13 +2399,13 @@
         <v>5004</v>
       </c>
       <c r="B86" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C86" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D86" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.2">
@@ -2410,13 +2413,13 @@
         <v>5004</v>
       </c>
       <c r="B87" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C87" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D87" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
@@ -2424,13 +2427,13 @@
         <v>5004</v>
       </c>
       <c r="B88" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D88" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.2">
@@ -2438,13 +2441,13 @@
         <v>5004</v>
       </c>
       <c r="B89" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C89" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D89" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
@@ -2452,13 +2455,13 @@
         <v>5004</v>
       </c>
       <c r="B90" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C90" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D90" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "Add enhanced parsing and vocabulary engines"
This reverts commit 931dc73d97c78f10676c085ad948cccb63f58682.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元.xlsx
+++ b/training/data/例文入力元.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\例文セットDB作成システム\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F325D64B-B662-4A25-A5C9-B1ACA0835D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A50ACA-91A0-4C90-B4A7-AE9E00964397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="3930" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,10 +230,19 @@
     <t>ex022</t>
   </si>
   <si>
+    <t>Would I hold the call, please?</t>
+  </si>
+  <si>
     <t>ex023</t>
   </si>
   <si>
+    <t>Would she hold the phone, please?</t>
+  </si>
+  <si>
     <t>ex024</t>
+  </si>
+  <si>
+    <t>Would they hold the connection, please?</t>
   </si>
   <si>
     <t>ex025</t>
@@ -680,18 +689,6 @@
   </si>
   <si>
     <t>discuss</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Would you hold the call, please?</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Would you hold the phone, please?</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Would you hold the connection, please?</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1100,7 +1097,7 @@
   <dimension ref="A1:V245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1289,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1306,7 +1303,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -1320,7 +1317,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1334,7 +1331,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -1348,7 +1345,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1362,7 +1359,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -1376,7 +1373,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -1390,7 +1387,7 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -1404,7 +1401,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1418,7 +1415,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1432,7 +1429,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1446,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1460,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -1474,7 +1471,7 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
@@ -1488,7 +1485,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D21" t="s">
         <v>55</v>
@@ -1502,7 +1499,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -1516,7 +1513,7 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1530,7 +1527,7 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -1544,7 +1541,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -1558,7 +1555,7 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
@@ -1572,7 +1569,7 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
@@ -1586,10 +1583,10 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D28" t="s">
-        <v>213</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -1597,13 +1594,13 @@
         <v>5004</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>214</v>
+        <v>71</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="4"/>
@@ -1613,13 +1610,13 @@
         <v>5004</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D30" t="s">
-        <v>215</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1627,13 +1624,13 @@
         <v>5004</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -1641,13 +1638,13 @@
         <v>5004</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -1655,13 +1652,13 @@
         <v>5004</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -1669,13 +1666,13 @@
         <v>5004</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -1683,13 +1680,13 @@
         <v>5004</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -1697,13 +1694,13 @@
         <v>5004</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -1711,13 +1708,13 @@
         <v>5004</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="V37" s="4"/>
     </row>
@@ -1726,13 +1723,13 @@
         <v>5004</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -1740,13 +1737,13 @@
         <v>5004</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -1754,13 +1751,13 @@
         <v>5004</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -1768,13 +1765,13 @@
         <v>5004</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -1782,13 +1779,13 @@
         <v>5004</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
@@ -1796,13 +1793,13 @@
         <v>5004</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -1810,13 +1807,13 @@
         <v>5004</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -1824,13 +1821,13 @@
         <v>5004</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -1838,13 +1835,13 @@
         <v>5004</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -1852,13 +1849,13 @@
         <v>5004</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -1866,13 +1863,13 @@
         <v>5004</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -1880,13 +1877,13 @@
         <v>5004</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D49" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -1894,13 +1891,13 @@
         <v>5004</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
@@ -1908,13 +1905,13 @@
         <v>5004</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -1922,13 +1919,13 @@
         <v>5004</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -1936,13 +1933,13 @@
         <v>5004</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D53" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -1950,13 +1947,13 @@
         <v>5004</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
@@ -1964,13 +1961,13 @@
         <v>5004</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
@@ -1978,13 +1975,13 @@
         <v>5004</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C56" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="V56" s="4"/>
     </row>
@@ -1993,13 +1990,13 @@
         <v>5004</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -2007,13 +2004,13 @@
         <v>5004</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D58" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -2021,13 +2018,13 @@
         <v>5004</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
@@ -2035,13 +2032,13 @@
         <v>5004</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
@@ -2049,13 +2046,13 @@
         <v>5004</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C61" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -2063,13 +2060,13 @@
         <v>5004</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D62" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -2077,13 +2074,13 @@
         <v>5004</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D63" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -2091,13 +2088,13 @@
         <v>5004</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C64" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D64" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2105,13 +2102,13 @@
         <v>5004</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D65" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2119,13 +2116,13 @@
         <v>5004</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D66" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2133,13 +2130,13 @@
         <v>5004</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C67" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2147,13 +2144,13 @@
         <v>5004</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2161,13 +2158,13 @@
         <v>5004</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2175,13 +2172,13 @@
         <v>5004</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C70" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2189,13 +2186,13 @@
         <v>5004</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C71" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D71" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2203,13 +2200,13 @@
         <v>5004</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D72" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2217,13 +2214,13 @@
         <v>5004</v>
       </c>
       <c r="B73" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C73" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2231,13 +2228,13 @@
         <v>5004</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2245,13 +2242,13 @@
         <v>5004</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C75" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2259,13 +2256,13 @@
         <v>5004</v>
       </c>
       <c r="B76" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C76" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D76" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2273,13 +2270,13 @@
         <v>5004</v>
       </c>
       <c r="B77" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C77" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D77" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2287,13 +2284,13 @@
         <v>5004</v>
       </c>
       <c r="B78" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C78" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D78" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2301,13 +2298,13 @@
         <v>5004</v>
       </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C79" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2315,13 +2312,13 @@
         <v>5004</v>
       </c>
       <c r="B80" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C80" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D80" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.2">
@@ -2329,13 +2326,13 @@
         <v>5004</v>
       </c>
       <c r="B81" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C81" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.2">
@@ -2343,13 +2340,13 @@
         <v>5004</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C82" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D82" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.2">
@@ -2357,13 +2354,13 @@
         <v>5004</v>
       </c>
       <c r="B83" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C83" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D83" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
@@ -2371,13 +2368,13 @@
         <v>5004</v>
       </c>
       <c r="B84" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C84" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D84" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.2">
@@ -2385,13 +2382,13 @@
         <v>5004</v>
       </c>
       <c r="B85" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C85" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D85" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
@@ -2399,13 +2396,13 @@
         <v>5004</v>
       </c>
       <c r="B86" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C86" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D86" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.2">
@@ -2413,13 +2410,13 @@
         <v>5004</v>
       </c>
       <c r="B87" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C87" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D87" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
@@ -2427,13 +2424,13 @@
         <v>5004</v>
       </c>
       <c r="B88" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C88" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D88" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.2">
@@ -2441,13 +2438,13 @@
         <v>5004</v>
       </c>
       <c r="B89" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C89" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D89" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
@@ -2455,13 +2452,13 @@
         <v>5004</v>
       </c>
       <c r="B90" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C90" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D90" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Handle perfect tense contractions and expand preposition checks
Added support for detecting perfect tense contractions (e.g., haven't, hasn't, hadn't) in RephraseParsingEngine. Expanded prepositional phrase detection to include more prepositions. Added a test script for parsing 'I haven't seen you for a long time.' Updated Excel data file.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元.xlsx
+++ b/training/data/例文入力元.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\例文セットDB作成システム\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A50ACA-91A0-4C90-B4A7-AE9E00964397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D547500E-E5C8-40BC-A1A9-BF84DCDABD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="3930" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,19 +230,10 @@
     <t>ex022</t>
   </si>
   <si>
-    <t>Would I hold the call, please?</t>
-  </si>
-  <si>
     <t>ex023</t>
   </si>
   <si>
-    <t>Would she hold the phone, please?</t>
-  </si>
-  <si>
     <t>ex024</t>
-  </si>
-  <si>
-    <t>Would they hold the connection, please?</t>
   </si>
   <si>
     <t>ex025</t>
@@ -689,6 +680,18 @@
   </si>
   <si>
     <t>discuss</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Would you hold the call, please?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Would you hold the phone, please?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Would you hold the connection, please?</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1289,7 +1292,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1303,7 +1306,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -1317,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1331,7 +1334,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -1345,7 +1348,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1359,7 +1362,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -1373,7 +1376,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -1387,7 +1390,7 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -1401,7 +1404,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1415,7 +1418,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1429,7 +1432,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1443,7 +1446,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1457,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -1471,7 +1474,7 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
@@ -1485,7 +1488,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
         <v>55</v>
@@ -1499,7 +1502,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -1513,7 +1516,7 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1527,7 +1530,7 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -1541,7 +1544,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -1555,7 +1558,7 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
@@ -1569,7 +1572,7 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
@@ -1583,10 +1586,10 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -1594,13 +1597,13 @@
         <v>5004</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>214</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="4"/>
@@ -1610,13 +1613,13 @@
         <v>5004</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1624,13 +1627,13 @@
         <v>5004</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -1638,13 +1641,13 @@
         <v>5004</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -1652,13 +1655,13 @@
         <v>5004</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -1666,13 +1669,13 @@
         <v>5004</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -1680,13 +1683,13 @@
         <v>5004</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -1694,13 +1697,13 @@
         <v>5004</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -1708,13 +1711,13 @@
         <v>5004</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V37" s="4"/>
     </row>
@@ -1723,13 +1726,13 @@
         <v>5004</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -1737,13 +1740,13 @@
         <v>5004</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -1751,13 +1754,13 @@
         <v>5004</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -1765,13 +1768,13 @@
         <v>5004</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -1779,13 +1782,13 @@
         <v>5004</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
@@ -1793,13 +1796,13 @@
         <v>5004</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -1807,13 +1810,13 @@
         <v>5004</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -1821,13 +1824,13 @@
         <v>5004</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -1835,13 +1838,13 @@
         <v>5004</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -1849,13 +1852,13 @@
         <v>5004</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -1863,13 +1866,13 @@
         <v>5004</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -1877,13 +1880,13 @@
         <v>5004</v>
       </c>
       <c r="B49" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -1891,13 +1894,13 @@
         <v>5004</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
@@ -1905,13 +1908,13 @@
         <v>5004</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D51" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -1919,13 +1922,13 @@
         <v>5004</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -1933,13 +1936,13 @@
         <v>5004</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -1947,13 +1950,13 @@
         <v>5004</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D54" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
@@ -1961,13 +1964,13 @@
         <v>5004</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D55" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
@@ -1975,13 +1978,13 @@
         <v>5004</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="V56" s="4"/>
     </row>
@@ -1990,13 +1993,13 @@
         <v>5004</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D57" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -2004,13 +2007,13 @@
         <v>5004</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D58" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -2018,13 +2021,13 @@
         <v>5004</v>
       </c>
       <c r="B59" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
@@ -2032,13 +2035,13 @@
         <v>5004</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C60" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D60" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
@@ -2046,13 +2049,13 @@
         <v>5004</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D61" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -2060,13 +2063,13 @@
         <v>5004</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C62" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D62" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -2074,13 +2077,13 @@
         <v>5004</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C63" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D63" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -2088,13 +2091,13 @@
         <v>5004</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2102,13 +2105,13 @@
         <v>5004</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2116,13 +2119,13 @@
         <v>5004</v>
       </c>
       <c r="B66" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C66" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2130,13 +2133,13 @@
         <v>5004</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2144,13 +2147,13 @@
         <v>5004</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D68" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2158,13 +2161,13 @@
         <v>5004</v>
       </c>
       <c r="B69" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D69" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2172,13 +2175,13 @@
         <v>5004</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D70" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2186,13 +2189,13 @@
         <v>5004</v>
       </c>
       <c r="B71" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2200,13 +2203,13 @@
         <v>5004</v>
       </c>
       <c r="B72" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C72" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D72" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2214,13 +2217,13 @@
         <v>5004</v>
       </c>
       <c r="B73" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D73" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2228,13 +2231,13 @@
         <v>5004</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D74" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2242,13 +2245,13 @@
         <v>5004</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D75" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2256,13 +2259,13 @@
         <v>5004</v>
       </c>
       <c r="B76" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C76" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D76" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2270,13 +2273,13 @@
         <v>5004</v>
       </c>
       <c r="B77" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D77" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2284,13 +2287,13 @@
         <v>5004</v>
       </c>
       <c r="B78" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D78" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2298,13 +2301,13 @@
         <v>5004</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D79" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2312,13 +2315,13 @@
         <v>5004</v>
       </c>
       <c r="B80" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.2">
@@ -2326,13 +2329,13 @@
         <v>5004</v>
       </c>
       <c r="B81" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C81" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.2">
@@ -2340,13 +2343,13 @@
         <v>5004</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C82" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D82" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.2">
@@ -2354,13 +2357,13 @@
         <v>5004</v>
       </c>
       <c r="B83" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C83" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D83" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
@@ -2368,13 +2371,13 @@
         <v>5004</v>
       </c>
       <c r="B84" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C84" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D84" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.2">
@@ -2382,13 +2385,13 @@
         <v>5004</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C85" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D85" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
@@ -2396,13 +2399,13 @@
         <v>5004</v>
       </c>
       <c r="B86" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C86" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D86" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.2">
@@ -2410,13 +2413,13 @@
         <v>5004</v>
       </c>
       <c r="B87" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C87" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D87" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
@@ -2424,13 +2427,13 @@
         <v>5004</v>
       </c>
       <c r="B88" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C88" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D88" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.2">
@@ -2438,13 +2441,13 @@
         <v>5004</v>
       </c>
       <c r="B89" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C89" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D89" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
@@ -2452,13 +2455,13 @@
         <v>5004</v>
       </c>
       <c r="B90" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C90" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D90" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactor slot order logic and add quality checks
Refactored Excel_Generator.py to compute slot display order per sentence based on phrase position, including contraction restoration. Added order_integrity_check.py and quality_checker.py scripts for validating slot order and contraction handling in generated Excel data. Added temp_data.csv and temp_fixed.csv for test and validation purposes.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元.xlsx
+++ b/training/data/例文入力元.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D547500E-E5C8-40BC-A1A9-BF84DCDABD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCDDE29-FBF4-41E8-A878-F376CEB56EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3870" yWindow="3930" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,9 +509,6 @@
     <t>ex070</t>
   </si>
   <si>
-    <t>He married a quiet woman.</t>
-  </si>
-  <si>
     <t>ex071</t>
   </si>
   <si>
@@ -521,9 +518,6 @@
     <t>ex072</t>
   </si>
   <si>
-    <t>They married their partners.</t>
-  </si>
-  <si>
     <t>ex073</t>
   </si>
   <si>
@@ -692,6 +686,14 @@
   </si>
   <si>
     <t>Would you hold the connection, please?</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Mary married a quiet guy.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>She married her partner.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1099,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1294,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1306,7 +1308,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -1320,7 +1322,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1334,7 +1336,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -1348,7 +1350,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1362,7 +1364,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -1376,7 +1378,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -1390,7 +1392,7 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -1404,7 +1406,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1418,7 +1420,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1432,7 +1434,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1446,7 +1448,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1460,7 +1462,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -1474,7 +1476,7 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
@@ -1488,7 +1490,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
         <v>55</v>
@@ -1502,7 +1504,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -1516,7 +1518,7 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1530,7 +1532,7 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -1544,7 +1546,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -1558,7 +1560,7 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
@@ -1572,7 +1574,7 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
@@ -1586,10 +1588,10 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -1600,10 +1602,10 @@
         <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="4"/>
@@ -1616,10 +1618,10 @@
         <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1630,7 +1632,7 @@
         <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D31" t="s">
         <v>72</v>
@@ -1644,7 +1646,7 @@
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D32" t="s">
         <v>74</v>
@@ -1658,7 +1660,7 @@
         <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D33" t="s">
         <v>76</v>
@@ -1672,7 +1674,7 @@
         <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D34" t="s">
         <v>78</v>
@@ -1686,7 +1688,7 @@
         <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D35" t="s">
         <v>80</v>
@@ -1700,7 +1702,7 @@
         <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D36" t="s">
         <v>82</v>
@@ -1714,7 +1716,7 @@
         <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D37" t="s">
         <v>84</v>
@@ -1729,7 +1731,7 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D38" t="s">
         <v>86</v>
@@ -1743,7 +1745,7 @@
         <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D39" t="s">
         <v>88</v>
@@ -1757,7 +1759,7 @@
         <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D40" t="s">
         <v>90</v>
@@ -1771,7 +1773,7 @@
         <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D41" t="s">
         <v>92</v>
@@ -1785,7 +1787,7 @@
         <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D42" t="s">
         <v>94</v>
@@ -1799,7 +1801,7 @@
         <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D43" t="s">
         <v>96</v>
@@ -1813,7 +1815,7 @@
         <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D44" t="s">
         <v>98</v>
@@ -1827,7 +1829,7 @@
         <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D45" t="s">
         <v>100</v>
@@ -1841,7 +1843,7 @@
         <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D46" t="s">
         <v>102</v>
@@ -1855,7 +1857,7 @@
         <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D47" t="s">
         <v>104</v>
@@ -1869,7 +1871,7 @@
         <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D48" t="s">
         <v>106</v>
@@ -1883,7 +1885,7 @@
         <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D49" t="s">
         <v>108</v>
@@ -1897,7 +1899,7 @@
         <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D50" t="s">
         <v>110</v>
@@ -1911,7 +1913,7 @@
         <v>111</v>
       </c>
       <c r="C51" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D51" t="s">
         <v>112</v>
@@ -1925,7 +1927,7 @@
         <v>113</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D52" t="s">
         <v>114</v>
@@ -1939,7 +1941,7 @@
         <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D53" t="s">
         <v>116</v>
@@ -1953,7 +1955,7 @@
         <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D54" t="s">
         <v>118</v>
@@ -1967,7 +1969,7 @@
         <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D55" t="s">
         <v>120</v>
@@ -1981,7 +1983,7 @@
         <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D56" t="s">
         <v>122</v>
@@ -1996,7 +1998,7 @@
         <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D57" t="s">
         <v>124</v>
@@ -2010,7 +2012,7 @@
         <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D58" t="s">
         <v>126</v>
@@ -2024,7 +2026,7 @@
         <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D59" t="s">
         <v>128</v>
@@ -2038,7 +2040,7 @@
         <v>129</v>
       </c>
       <c r="C60" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D60" t="s">
         <v>130</v>
@@ -2052,7 +2054,7 @@
         <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D61" t="s">
         <v>132</v>
@@ -2066,7 +2068,7 @@
         <v>133</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D62" t="s">
         <v>134</v>
@@ -2080,7 +2082,7 @@
         <v>135</v>
       </c>
       <c r="C63" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D63" t="s">
         <v>136</v>
@@ -2094,7 +2096,7 @@
         <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D64" t="s">
         <v>138</v>
@@ -2108,7 +2110,7 @@
         <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D65" t="s">
         <v>140</v>
@@ -2122,7 +2124,7 @@
         <v>141</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D66" t="s">
         <v>142</v>
@@ -2136,7 +2138,7 @@
         <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D67" t="s">
         <v>144</v>
@@ -2150,7 +2152,7 @@
         <v>145</v>
       </c>
       <c r="C68" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D68" t="s">
         <v>146</v>
@@ -2164,7 +2166,7 @@
         <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D69" t="s">
         <v>148</v>
@@ -2178,7 +2180,7 @@
         <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D70" t="s">
         <v>150</v>
@@ -2192,7 +2194,7 @@
         <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D71" t="s">
         <v>152</v>
@@ -2206,7 +2208,7 @@
         <v>153</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D72" t="s">
         <v>154</v>
@@ -2220,7 +2222,7 @@
         <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D73" t="s">
         <v>156</v>
@@ -2234,7 +2236,7 @@
         <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D74" t="s">
         <v>158</v>
@@ -2248,7 +2250,7 @@
         <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D75" t="s">
         <v>160</v>
@@ -2262,10 +2264,10 @@
         <v>161</v>
       </c>
       <c r="C76" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D76" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2273,13 +2275,13 @@
         <v>5004</v>
       </c>
       <c r="B77" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" t="s">
+        <v>207</v>
+      </c>
+      <c r="D77" t="s">
         <v>163</v>
-      </c>
-      <c r="C77" t="s">
-        <v>209</v>
-      </c>
-      <c r="D77" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2287,13 +2289,13 @@
         <v>5004</v>
       </c>
       <c r="B78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C78" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D78" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2301,13 +2303,13 @@
         <v>5004</v>
       </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2315,13 +2317,13 @@
         <v>5004</v>
       </c>
       <c r="B80" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C80" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D80" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.2">
@@ -2329,13 +2331,13 @@
         <v>5004</v>
       </c>
       <c r="B81" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C81" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.2">
@@ -2343,13 +2345,13 @@
         <v>5004</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C82" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D82" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.2">
@@ -2357,13 +2359,13 @@
         <v>5004</v>
       </c>
       <c r="B83" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C83" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D83" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
@@ -2371,13 +2373,13 @@
         <v>5004</v>
       </c>
       <c r="B84" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C84" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.2">
@@ -2385,13 +2387,13 @@
         <v>5004</v>
       </c>
       <c r="B85" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C85" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D85" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
@@ -2399,13 +2401,13 @@
         <v>5004</v>
       </c>
       <c r="B86" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C86" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D86" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.2">
@@ -2413,13 +2415,13 @@
         <v>5004</v>
       </c>
       <c r="B87" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C87" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D87" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
@@ -2427,13 +2429,13 @@
         <v>5004</v>
       </c>
       <c r="B88" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C88" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D88" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.2">
@@ -2441,13 +2443,13 @@
         <v>5004</v>
       </c>
       <c r="B89" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C89" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D89" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
@@ -2455,13 +2457,13 @@
         <v>5004</v>
       </c>
       <c r="B90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C90" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D90" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add Excel generator and parsing engine scripts
Added new Python scripts for generating Excel files from sentence parsing results (Excel_Generator.py, Excel_Generator_v2.py), a comprehensive parsing engine (Rephrase_Parsing_Engine.py), and supporting data files (quality_verification.py, rephrase_rules_v1.0.json, sample_sentences.txt, and slot order data). Also updated index.html with a minor change to the file ending.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元.xlsx
+++ b/training/data/例文入力元.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\完全トレーニングUI完成フェーズ３\project-root\Rephrase-Project\training\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurit\Downloads\Rephraseプロジェクト20250529\例文セットDB作成システム\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCDDE29-FBF4-41E8-A878-F376CEB56EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A50ACA-91A0-4C90-B4A7-AE9E00964397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="3930" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="33490" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,12 +230,21 @@
     <t>ex022</t>
   </si>
   <si>
+    <t>Would I hold the call, please?</t>
+  </si>
+  <si>
     <t>ex023</t>
   </si>
   <si>
+    <t>Would she hold the phone, please?</t>
+  </si>
+  <si>
     <t>ex024</t>
   </si>
   <si>
+    <t>Would they hold the connection, please?</t>
+  </si>
+  <si>
     <t>ex025</t>
   </si>
   <si>
@@ -509,6 +518,9 @@
     <t>ex070</t>
   </si>
   <si>
+    <t>He married a quiet woman.</t>
+  </si>
+  <si>
     <t>ex071</t>
   </si>
   <si>
@@ -516,6 +528,9 @@
   </si>
   <si>
     <t>ex072</t>
+  </si>
+  <si>
+    <t>They married their partners.</t>
   </si>
   <si>
     <t>ex073</t>
@@ -674,26 +689,6 @@
   </si>
   <si>
     <t>discuss</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Would you hold the call, please?</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Would you hold the phone, please?</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Would you hold the connection, please?</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Mary married a quiet guy.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>She married her partner.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1101,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1289,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -1308,7 +1303,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -1322,7 +1317,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1336,7 +1331,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -1350,7 +1345,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1364,7 +1359,7 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -1378,7 +1373,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -1392,7 +1387,7 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -1406,7 +1401,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1420,7 +1415,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1434,7 +1429,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1448,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1462,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -1476,7 +1471,7 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
@@ -1490,7 +1485,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D21" t="s">
         <v>55</v>
@@ -1504,7 +1499,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -1518,7 +1513,7 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1532,7 +1527,7 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
@@ -1546,7 +1541,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -1560,7 +1555,7 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
@@ -1574,7 +1569,7 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
@@ -1588,10 +1583,10 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D28" t="s">
-        <v>211</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -1599,13 +1594,13 @@
         <v>5004</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>212</v>
+        <v>71</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="4"/>
@@ -1615,13 +1610,13 @@
         <v>5004</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1629,13 +1624,13 @@
         <v>5004</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -1643,13 +1638,13 @@
         <v>5004</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -1657,13 +1652,13 @@
         <v>5004</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -1671,13 +1666,13 @@
         <v>5004</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -1685,13 +1680,13 @@
         <v>5004</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
@@ -1699,13 +1694,13 @@
         <v>5004</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -1713,13 +1708,13 @@
         <v>5004</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="V37" s="4"/>
     </row>
@@ -1728,13 +1723,13 @@
         <v>5004</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -1742,13 +1737,13 @@
         <v>5004</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -1756,13 +1751,13 @@
         <v>5004</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -1770,13 +1765,13 @@
         <v>5004</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -1784,13 +1779,13 @@
         <v>5004</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
@@ -1798,13 +1793,13 @@
         <v>5004</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -1812,13 +1807,13 @@
         <v>5004</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -1826,13 +1821,13 @@
         <v>5004</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -1840,13 +1835,13 @@
         <v>5004</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -1854,13 +1849,13 @@
         <v>5004</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -1868,13 +1863,13 @@
         <v>5004</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -1882,13 +1877,13 @@
         <v>5004</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C49" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D49" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
@@ -1896,13 +1891,13 @@
         <v>5004</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
@@ -1910,13 +1905,13 @@
         <v>5004</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -1924,13 +1919,13 @@
         <v>5004</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -1938,13 +1933,13 @@
         <v>5004</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D53" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -1952,13 +1947,13 @@
         <v>5004</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
@@ -1966,13 +1961,13 @@
         <v>5004</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
@@ -1980,13 +1975,13 @@
         <v>5004</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C56" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="V56" s="4"/>
     </row>
@@ -1995,13 +1990,13 @@
         <v>5004</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -2009,13 +2004,13 @@
         <v>5004</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C58" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D58" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -2023,13 +2018,13 @@
         <v>5004</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
@@ -2037,13 +2032,13 @@
         <v>5004</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
@@ -2051,13 +2046,13 @@
         <v>5004</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C61" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -2065,13 +2060,13 @@
         <v>5004</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C62" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D62" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -2079,13 +2074,13 @@
         <v>5004</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D63" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -2093,13 +2088,13 @@
         <v>5004</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C64" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D64" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2107,13 +2102,13 @@
         <v>5004</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D65" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2121,13 +2116,13 @@
         <v>5004</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D66" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2135,13 +2130,13 @@
         <v>5004</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2149,13 +2144,13 @@
         <v>5004</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2163,13 +2158,13 @@
         <v>5004</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2177,13 +2172,13 @@
         <v>5004</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C70" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2191,13 +2186,13 @@
         <v>5004</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C71" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D71" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2205,13 +2200,13 @@
         <v>5004</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C72" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D72" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2219,13 +2214,13 @@
         <v>5004</v>
       </c>
       <c r="B73" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C73" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2233,13 +2228,13 @@
         <v>5004</v>
       </c>
       <c r="B74" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2247,13 +2242,13 @@
         <v>5004</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C75" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2261,13 +2256,13 @@
         <v>5004</v>
       </c>
       <c r="B76" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C76" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D76" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2275,13 +2270,13 @@
         <v>5004</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C77" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2289,13 +2284,13 @@
         <v>5004</v>
       </c>
       <c r="B78" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C78" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D78" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2303,13 +2298,13 @@
         <v>5004</v>
       </c>
       <c r="B79" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C79" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D79" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2317,13 +2312,13 @@
         <v>5004</v>
       </c>
       <c r="B80" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C80" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D80" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.2">
@@ -2331,13 +2326,13 @@
         <v>5004</v>
       </c>
       <c r="B81" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C81" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D81" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.2">
@@ -2345,13 +2340,13 @@
         <v>5004</v>
       </c>
       <c r="B82" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C82" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D82" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.2">
@@ -2359,13 +2354,13 @@
         <v>5004</v>
       </c>
       <c r="B83" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C83" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D83" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
@@ -2373,13 +2368,13 @@
         <v>5004</v>
       </c>
       <c r="B84" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C84" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D84" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.2">
@@ -2387,13 +2382,13 @@
         <v>5004</v>
       </c>
       <c r="B85" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C85" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D85" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
@@ -2401,13 +2396,13 @@
         <v>5004</v>
       </c>
       <c r="B86" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C86" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D86" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.2">
@@ -2415,13 +2410,13 @@
         <v>5004</v>
       </c>
       <c r="B87" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C87" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D87" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
@@ -2429,13 +2424,13 @@
         <v>5004</v>
       </c>
       <c r="B88" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C88" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D88" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.2">
@@ -2443,13 +2438,13 @@
         <v>5004</v>
       </c>
       <c r="B89" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C89" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D89" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
@@ -2457,13 +2452,13 @@
         <v>5004</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C90" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D90" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>